<commit_message>
roadmap and schedule updated. dev begins
</commit_message>
<xml_diff>
--- a/docs/Cronograma.xlsx
+++ b/docs/Cronograma.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\urielf\Documents\CPTM\DEV\GPR\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\urielf\Documents\CPTM\DEV\GRD\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8E2144-FA05-4623-878C-B5F34DF55464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21990F2B-9C08-4C32-9F3D-3C2F0A4E3075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectSchedule" sheetId="11" r:id="rId1"/>
@@ -916,11 +916,8 @@
     <xf numFmtId="168" fontId="5" fillId="10" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -931,8 +928,11 @@
     <xf numFmtId="165" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1495,24 +1495,24 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="10.42578125" style="5" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" customWidth="1"/>
-    <col min="8" max="8" width="6.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="64" width="2.5703125" customWidth="1"/>
-    <col min="69" max="70" width="10.28515625"/>
+    <col min="1" max="1" width="2.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.44140625" style="5" customWidth="1"/>
+    <col min="6" max="6" width="10.44140625" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
+    <col min="8" max="8" width="6.109375" hidden="1" customWidth="1"/>
+    <col min="9" max="64" width="2.5546875" customWidth="1"/>
+    <col min="69" max="70" width="10.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:64" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="16" t="s">
         <v>21</v>
       </c>
@@ -1522,141 +1522,141 @@
       <c r="F1" s="76"/>
       <c r="H1" s="2"/>
       <c r="I1" s="8"/>
-      <c r="J1" s="98" t="str">
+      <c r="J1" s="93" t="str">
         <f>HYPERLINK("https://vertex42.link/HowToMakeAGanttChart","► Watch How to Make a Gantt Chart in Excel")</f>
         <v>► Watch How to Make a Gantt Chart in Excel</v>
       </c>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="98"/>
-      <c r="R1" s="98"/>
-      <c r="S1" s="98"/>
-      <c r="T1" s="98"/>
-      <c r="U1" s="98"/>
-      <c r="V1" s="98"/>
-      <c r="W1" s="98"/>
-      <c r="X1" s="98"/>
-      <c r="Y1" s="98"/>
-      <c r="Z1" s="98"/>
-      <c r="AA1" s="98"/>
-    </row>
-    <row r="2" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K1" s="93"/>
+      <c r="L1" s="93"/>
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="93"/>
+      <c r="P1" s="93"/>
+      <c r="Q1" s="93"/>
+      <c r="R1" s="93"/>
+      <c r="S1" s="93"/>
+      <c r="T1" s="93"/>
+      <c r="U1" s="93"/>
+      <c r="V1" s="93"/>
+      <c r="W1" s="93"/>
+      <c r="X1" s="93"/>
+      <c r="Y1" s="93"/>
+      <c r="Z1" s="93"/>
+      <c r="AA1" s="93"/>
+    </row>
+    <row r="2" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
         <v>17</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="93">
+      <c r="E2" s="97">
         <v>44733</v>
       </c>
-      <c r="F2" s="94"/>
-    </row>
-    <row r="3" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="98"/>
+    </row>
+    <row r="3" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="9" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="93">
+      <c r="E3" s="97">
         <v>43474</v>
       </c>
-      <c r="F3" s="94"/>
-    </row>
-    <row r="4" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F3" s="98"/>
+    </row>
+    <row r="4" spans="1:64" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D4" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E4" s="7">
         <v>1</v>
       </c>
-      <c r="I4" s="95">
+      <c r="I4" s="94">
         <f>I5</f>
         <v>44732</v>
       </c>
-      <c r="J4" s="96"/>
-      <c r="K4" s="96"/>
-      <c r="L4" s="96"/>
-      <c r="M4" s="96"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="97"/>
-      <c r="P4" s="95">
+      <c r="J4" s="95"/>
+      <c r="K4" s="95"/>
+      <c r="L4" s="95"/>
+      <c r="M4" s="95"/>
+      <c r="N4" s="95"/>
+      <c r="O4" s="96"/>
+      <c r="P4" s="94">
         <f>P5</f>
         <v>44739</v>
       </c>
-      <c r="Q4" s="96"/>
-      <c r="R4" s="96"/>
-      <c r="S4" s="96"/>
-      <c r="T4" s="96"/>
-      <c r="U4" s="96"/>
-      <c r="V4" s="97"/>
-      <c r="W4" s="95">
+      <c r="Q4" s="95"/>
+      <c r="R4" s="95"/>
+      <c r="S4" s="95"/>
+      <c r="T4" s="95"/>
+      <c r="U4" s="95"/>
+      <c r="V4" s="96"/>
+      <c r="W4" s="94">
         <f>W5</f>
         <v>44746</v>
       </c>
-      <c r="X4" s="96"/>
-      <c r="Y4" s="96"/>
-      <c r="Z4" s="96"/>
-      <c r="AA4" s="96"/>
-      <c r="AB4" s="96"/>
-      <c r="AC4" s="97"/>
-      <c r="AD4" s="95">
+      <c r="X4" s="95"/>
+      <c r="Y4" s="95"/>
+      <c r="Z4" s="95"/>
+      <c r="AA4" s="95"/>
+      <c r="AB4" s="95"/>
+      <c r="AC4" s="96"/>
+      <c r="AD4" s="94">
         <f>AD5</f>
         <v>44753</v>
       </c>
-      <c r="AE4" s="96"/>
-      <c r="AF4" s="96"/>
-      <c r="AG4" s="96"/>
-      <c r="AH4" s="96"/>
-      <c r="AI4" s="96"/>
-      <c r="AJ4" s="97"/>
-      <c r="AK4" s="95">
+      <c r="AE4" s="95"/>
+      <c r="AF4" s="95"/>
+      <c r="AG4" s="95"/>
+      <c r="AH4" s="95"/>
+      <c r="AI4" s="95"/>
+      <c r="AJ4" s="96"/>
+      <c r="AK4" s="94">
         <f>AK5</f>
         <v>44760</v>
       </c>
-      <c r="AL4" s="96"/>
-      <c r="AM4" s="96"/>
-      <c r="AN4" s="96"/>
-      <c r="AO4" s="96"/>
-      <c r="AP4" s="96"/>
-      <c r="AQ4" s="97"/>
-      <c r="AR4" s="95">
+      <c r="AL4" s="95"/>
+      <c r="AM4" s="95"/>
+      <c r="AN4" s="95"/>
+      <c r="AO4" s="95"/>
+      <c r="AP4" s="95"/>
+      <c r="AQ4" s="96"/>
+      <c r="AR4" s="94">
         <f>AR5</f>
         <v>44767</v>
       </c>
-      <c r="AS4" s="96"/>
-      <c r="AT4" s="96"/>
-      <c r="AU4" s="96"/>
-      <c r="AV4" s="96"/>
-      <c r="AW4" s="96"/>
-      <c r="AX4" s="97"/>
-      <c r="AY4" s="95">
+      <c r="AS4" s="95"/>
+      <c r="AT4" s="95"/>
+      <c r="AU4" s="95"/>
+      <c r="AV4" s="95"/>
+      <c r="AW4" s="95"/>
+      <c r="AX4" s="96"/>
+      <c r="AY4" s="94">
         <f>AY5</f>
         <v>44774</v>
       </c>
-      <c r="AZ4" s="96"/>
-      <c r="BA4" s="96"/>
-      <c r="BB4" s="96"/>
-      <c r="BC4" s="96"/>
-      <c r="BD4" s="96"/>
-      <c r="BE4" s="97"/>
-      <c r="BF4" s="95">
+      <c r="AZ4" s="95"/>
+      <c r="BA4" s="95"/>
+      <c r="BB4" s="95"/>
+      <c r="BC4" s="95"/>
+      <c r="BD4" s="95"/>
+      <c r="BE4" s="96"/>
+      <c r="BF4" s="94">
         <f>BF5</f>
         <v>44781</v>
       </c>
-      <c r="BG4" s="96"/>
-      <c r="BH4" s="96"/>
-      <c r="BI4" s="96"/>
-      <c r="BJ4" s="96"/>
-      <c r="BK4" s="96"/>
-      <c r="BL4" s="97"/>
-    </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
+      <c r="BG4" s="95"/>
+      <c r="BH4" s="95"/>
+      <c r="BI4" s="95"/>
+      <c r="BJ4" s="95"/>
+      <c r="BK4" s="95"/>
+      <c r="BL4" s="96"/>
+    </row>
+    <row r="5" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="G5" s="6"/>
       <c r="I5" s="13">
@@ -1884,7 +1884,7 @@
         <v>44787</v>
       </c>
     </row>
-    <row r="6" spans="1:64" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:64" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="19"/>
       <c r="B6" s="10" t="s">
         <v>22</v>
@@ -2130,7 +2130,7 @@
         <v>d</v>
       </c>
     </row>
-    <row r="7" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="19"/>
       <c r="B7" s="20"/>
       <c r="C7" s="21"/>
@@ -2199,7 +2199,7 @@
       <c r="BK7" s="60"/>
       <c r="BL7" s="60"/>
     </row>
-    <row r="8" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="19"/>
       <c r="B8" s="26" t="s">
         <v>27</v>
@@ -2270,14 +2270,14 @@
       <c r="BK8" s="60"/>
       <c r="BL8" s="60"/>
     </row>
-    <row r="9" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="19"/>
       <c r="B9" s="31" t="s">
         <v>31</v>
       </c>
       <c r="C9" s="32"/>
       <c r="D9" s="33">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="E9" s="81">
         <v>44733</v>
@@ -2347,7 +2347,7 @@
       <c r="BK9" s="60"/>
       <c r="BL9" s="60"/>
     </row>
-    <row r="10" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="19"/>
       <c r="B10" s="31" t="s">
         <v>32</v>
@@ -2424,7 +2424,7 @@
       <c r="BK10" s="60"/>
       <c r="BL10" s="60"/>
     </row>
-    <row r="11" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="19"/>
       <c r="B11" s="31" t="s">
         <v>33</v>
@@ -2501,7 +2501,7 @@
       <c r="BK11" s="60"/>
       <c r="BL11" s="60"/>
     </row>
-    <row r="12" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="19"/>
       <c r="B12" s="34" t="s">
         <v>28</v>
@@ -2572,7 +2572,7 @@
       <c r="BK12" s="60"/>
       <c r="BL12" s="60"/>
     </row>
-    <row r="13" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="19"/>
       <c r="B13" s="39" t="s">
         <v>34</v>
@@ -2649,7 +2649,7 @@
       <c r="BK13" s="60"/>
       <c r="BL13" s="60"/>
     </row>
-    <row r="14" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="19"/>
       <c r="B14" s="39" t="s">
         <v>35</v>
@@ -2726,7 +2726,7 @@
       <c r="BK14" s="60"/>
       <c r="BL14" s="60"/>
     </row>
-    <row r="15" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="19"/>
       <c r="B15" s="39" t="s">
         <v>36</v>
@@ -2803,7 +2803,7 @@
       <c r="BK15" s="60"/>
       <c r="BL15" s="60"/>
     </row>
-    <row r="16" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="19"/>
       <c r="B16" s="42" t="s">
         <v>29</v>
@@ -2874,7 +2874,7 @@
       <c r="BK16" s="60"/>
       <c r="BL16" s="60"/>
     </row>
-    <row r="17" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="19"/>
       <c r="B17" s="45" t="s">
         <v>37</v>
@@ -2951,7 +2951,7 @@
       <c r="BK17" s="60"/>
       <c r="BL17" s="60"/>
     </row>
-    <row r="18" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="19"/>
       <c r="B18" s="45" t="s">
         <v>38</v>
@@ -3028,7 +3028,7 @@
       <c r="BK18" s="60"/>
       <c r="BL18" s="60"/>
     </row>
-    <row r="19" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="19"/>
       <c r="B19" s="48" t="s">
         <v>30</v>
@@ -3099,7 +3099,7 @@
       <c r="BK19" s="60"/>
       <c r="BL19" s="60"/>
     </row>
-    <row r="20" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="19"/>
       <c r="B20" s="51" t="s">
         <v>39</v>
@@ -3176,7 +3176,7 @@
       <c r="BK20" s="60"/>
       <c r="BL20" s="60"/>
     </row>
-    <row r="21" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="19"/>
       <c r="B21" s="51" t="s">
         <v>40</v>
@@ -3253,7 +3253,7 @@
       <c r="BK21" s="60"/>
       <c r="BL21" s="60"/>
     </row>
-    <row r="22" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="19"/>
       <c r="B22" s="20"/>
       <c r="C22" s="21"/>
@@ -3322,7 +3322,7 @@
       <c r="BK22" s="60"/>
       <c r="BL22" s="60"/>
     </row>
-    <row r="23" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="19"/>
       <c r="B23" s="20"/>
       <c r="C23" s="21"/>
@@ -3391,7 +3391,7 @@
       <c r="BK23" s="60"/>
       <c r="BL23" s="60"/>
     </row>
-    <row r="24" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="19"/>
       <c r="B24" s="20"/>
       <c r="C24" s="21"/>
@@ -3460,7 +3460,7 @@
       <c r="BK24" s="60"/>
       <c r="BL24" s="60"/>
     </row>
-    <row r="25" spans="1:64" s="3" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:64" s="3" customFormat="1" ht="21.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="19"/>
       <c r="B25" s="54" t="s">
         <v>0</v>
@@ -3531,11 +3531,11 @@
       <c r="BK25" s="62"/>
       <c r="BL25" s="62"/>
     </row>
-    <row r="26" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:64" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
       <c r="G26" s="6"/>
     </row>
-    <row r="27" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:64" x14ac:dyDescent="0.3">
       <c r="B27" s="17" t="s">
         <v>6</v>
       </c>
@@ -3544,30 +3544,30 @@
         <v>43113</v>
       </c>
     </row>
-    <row r="28" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:64" x14ac:dyDescent="0.3">
       <c r="B28" s="79" t="s">
         <v>11</v>
       </c>
       <c r="C28" s="18"/>
     </row>
-    <row r="29" spans="1:64" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:64" x14ac:dyDescent="0.3">
       <c r="B29" s="78" t="s">
         <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="J1:AA1"/>
-    <mergeCell ref="AK4:AQ4"/>
-    <mergeCell ref="AR4:AX4"/>
-    <mergeCell ref="AY4:BE4"/>
-    <mergeCell ref="BF4:BL4"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="I4:O4"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="AD4:AJ4"/>
     <mergeCell ref="E3:F3"/>
+    <mergeCell ref="J1:AA1"/>
+    <mergeCell ref="AK4:AQ4"/>
+    <mergeCell ref="AR4:AX4"/>
+    <mergeCell ref="AY4:BE4"/>
+    <mergeCell ref="BF4:BL4"/>
   </mergeCells>
   <conditionalFormatting sqref="D7:D25">
     <cfRule type="dataBar" priority="12">
@@ -3639,108 +3639,108 @@
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="64" customWidth="1"/>
-    <col min="2" max="2" width="87.140625" style="71" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="64"/>
+    <col min="1" max="1" width="2.88671875" style="64" customWidth="1"/>
+    <col min="2" max="2" width="87.109375" style="71" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="64"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:3" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="63"/>
     </row>
-    <row r="2" spans="2:3" s="66" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" s="66" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B2" s="65" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="65"/>
     </row>
-    <row r="3" spans="2:3" s="68" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" s="68" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="67" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="67"/>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="77" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="63"/>
     </row>
-    <row r="6" spans="2:3" s="69" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:3" s="69" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B6" s="72" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B7" s="73" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B8" s="70"/>
     </row>
-    <row r="9" spans="2:3" s="69" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:3" s="69" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B9" s="72" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="60" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B10" s="73" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B11" s="74" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B12" s="70"/>
     </row>
-    <row r="13" spans="2:3" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B13" s="80" t="str">
         <f>HYPERLINK("https://vertex42.link/HowToMakeAGanttChart","► Watch How This Gantt Chart Was Created")</f>
         <v>► Watch How This Gantt Chart Was Created</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:3" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B14" s="70"/>
     </row>
-    <row r="15" spans="2:3" s="69" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="15" spans="2:3" s="69" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B15" s="72" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="2:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B16" s="73" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:2" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B17" s="74" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B18" s="70"/>
     </row>
-    <row r="19" spans="2:2" s="69" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:2" s="69" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
       <c r="B19" s="72" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="2:2" ht="60" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B20" s="73" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="2:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:2" ht="14.4" x14ac:dyDescent="0.3">
       <c r="B21" s="70"/>
     </row>
-    <row r="22" spans="2:2" ht="75" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:2" ht="72" x14ac:dyDescent="0.3">
       <c r="B22" s="73" t="s">
         <v>10</v>
       </c>

</xml_diff>